<commit_message>
Relax bound on biofuel supply in transport
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_NCAP_2020.xlsx
+++ b/SuppXLS/Scen_TRA_NCAP_2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CD5780-EC46-45D3-865A-65C8C70A3746}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009D73EB-43FC-4089-B9E4-CFE3954EBE33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="244">
   <si>
     <t>Year</t>
   </si>
@@ -858,6 +858,9 @@
   <si>
     <t>*New</t>
   </si>
+  <si>
+    <t>Trans - Insert</t>
+  </si>
 </sst>
 </file>
 
@@ -866,8 +869,8 @@
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="0.0%"/>
-    <numFmt numFmtId="183" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -933,12 +936,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -958,11 +963,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1435,7 +1442,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
@@ -1445,7 +1452,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1455,12 +1462,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1482,6 +1486,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="273">
@@ -1801,7 +1808,7 @@
                   <a14:compatExt spid="_x0000_s11265"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C78FF535-BF42-4C38-B4AF-91371D0B12B9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000012C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1979,7 +1986,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3073,7 +3080,7 @@
   <dimension ref="A1:AH24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3094,6 +3101,11 @@
     </row>
     <row r="2" spans="1:34" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:34" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
+        <v>243</v>
+      </c>
+    </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -4563,13 +4575,13 @@
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="35">
         <v>2020</v>
       </c>
     </row>
@@ -4669,13 +4681,13 @@
       <c r="D17" s="12"/>
     </row>
     <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="36">
+      <c r="C18" s="35">
         <v>2020</v>
       </c>
       <c r="D18" s="13"/>
@@ -4797,13 +4809,13 @@
       <c r="C31" s="9"/>
     </row>
     <row r="32" spans="1:4" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="36">
+      <c r="C32" s="35">
         <v>2020</v>
       </c>
     </row>
@@ -5182,628 +5194,628 @@
       <c r="AC44" s="28"/>
     </row>
     <row r="49" spans="2:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="B49" s="35" t="s">
+      <c r="B49" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="C49" s="35"/>
+      <c r="C49" s="43"/>
     </row>
     <row r="50" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="37" t="s">
+      <c r="B50" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C50" s="37" t="s">
+      <c r="C50" s="36" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="38" t="s">
+      <c r="B51" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="C51" s="39"/>
+      <c r="C51" s="38"/>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B52" s="40" t="s">
+      <c r="B52" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="C52" s="40"/>
+      <c r="C52" s="39"/>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="C53" s="41" t="s">
+      <c r="C53" s="40" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B54" s="41" t="s">
+      <c r="B54" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="C54" s="41" t="s">
+      <c r="C54" s="40" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B55" s="40" t="s">
+      <c r="B55" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="C55" s="40"/>
+      <c r="C55" s="39"/>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B56" s="41" t="s">
+      <c r="B56" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="C56" s="41" t="s">
+      <c r="C56" s="40" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B57" s="41" t="s">
+      <c r="B57" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="41" t="s">
+      <c r="C57" s="40" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B58" s="41" t="s">
+      <c r="B58" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="C58" s="41" t="s">
+      <c r="C58" s="40" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B59" s="41" t="s">
+      <c r="B59" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="C59" s="41" t="s">
+      <c r="C59" s="40" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B60" s="41" t="s">
+      <c r="B60" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="C60" s="41" t="s">
+      <c r="C60" s="40" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B61" s="41" t="s">
+      <c r="B61" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="C61" s="41" t="s">
+      <c r="C61" s="40" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B62" s="41" t="s">
+      <c r="B62" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="C62" s="41" t="s">
+      <c r="C62" s="40" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B63" s="41" t="s">
+      <c r="B63" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="C63" s="41" t="s">
+      <c r="C63" s="40" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B64" s="41" t="s">
+      <c r="B64" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="C64" s="41" t="s">
+      <c r="C64" s="40" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B65" s="41" t="s">
+      <c r="B65" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="C65" s="41" t="s">
+      <c r="C65" s="40" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B66" s="41" t="s">
+      <c r="B66" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="C66" s="41" t="s">
+      <c r="C66" s="40" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B67" s="41" t="s">
+      <c r="B67" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C67" s="41" t="s">
+      <c r="C67" s="40" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B68" s="41" t="s">
+      <c r="B68" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="C68" s="41" t="s">
+      <c r="C68" s="40" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B69" s="41" t="s">
+      <c r="B69" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="C69" s="41" t="s">
+      <c r="C69" s="40" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B70" s="41" t="s">
+      <c r="B70" s="40" t="s">
         <v>128</v>
       </c>
-      <c r="C70" s="41" t="s">
+      <c r="C70" s="40" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B71" s="41" t="s">
+      <c r="B71" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="C71" s="41" t="s">
+      <c r="C71" s="40" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B72" s="41" t="s">
+      <c r="B72" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="C72" s="41" t="s">
+      <c r="C72" s="40" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B73" s="41" t="s">
+      <c r="B73" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="C73" s="41" t="s">
+      <c r="C73" s="40" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B74" s="41" t="s">
+      <c r="B74" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="C74" s="41" t="s">
+      <c r="C74" s="40" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B75" s="40" t="s">
+      <c r="B75" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="C75" s="40"/>
+      <c r="C75" s="39"/>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B76" s="41" t="s">
+      <c r="B76" s="40" t="s">
         <v>139</v>
       </c>
-      <c r="C76" s="41" t="s">
+      <c r="C76" s="40" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B77" s="41" t="s">
+      <c r="B77" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="C77" s="41" t="s">
+      <c r="C77" s="40" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B78" s="41" t="s">
+      <c r="B78" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="C78" s="41" t="s">
+      <c r="C78" s="40" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B79" s="41" t="s">
+      <c r="B79" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="C79" s="41" t="s">
+      <c r="C79" s="40" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B80" s="41" t="s">
+      <c r="B80" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="C80" s="41" t="s">
+      <c r="C80" s="40" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B81" s="41" t="s">
+      <c r="B81" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="C81" s="41" t="s">
+      <c r="C81" s="40" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B82" s="41" t="s">
+      <c r="B82" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="C82" s="41" t="s">
+      <c r="C82" s="40" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B83" s="41" t="s">
+      <c r="B83" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="C83" s="41" t="s">
+      <c r="C83" s="40" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B84" s="41" t="s">
+      <c r="B84" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="C84" s="41" t="s">
+      <c r="C84" s="40" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B85" s="41" t="s">
+      <c r="B85" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="C85" s="41" t="s">
+      <c r="C85" s="40" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B86" s="41" t="s">
+      <c r="B86" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="C86" s="41" t="s">
+      <c r="C86" s="40" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B87" s="41" t="s">
+      <c r="B87" s="40" t="s">
         <v>161</v>
       </c>
-      <c r="C87" s="41" t="s">
+      <c r="C87" s="40" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B88" s="41" t="s">
+      <c r="B88" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="C88" s="41" t="s">
+      <c r="C88" s="40" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B89" s="41" t="s">
+      <c r="B89" s="40" t="s">
         <v>165</v>
       </c>
-      <c r="C89" s="41" t="s">
+      <c r="C89" s="40" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B90" s="41" t="s">
+      <c r="B90" s="40" t="s">
         <v>167</v>
       </c>
-      <c r="C90" s="41" t="s">
+      <c r="C90" s="40" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B91" s="41" t="s">
+      <c r="B91" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="C91" s="41" t="s">
+      <c r="C91" s="40" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B92" s="41" t="s">
+      <c r="B92" s="40" t="s">
         <v>171</v>
       </c>
-      <c r="C92" s="41" t="s">
+      <c r="C92" s="40" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B93" s="41" t="s">
+      <c r="B93" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="C93" s="41" t="s">
+      <c r="C93" s="40" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B94" s="41" t="s">
+      <c r="B94" s="40" t="s">
         <v>175</v>
       </c>
-      <c r="C94" s="41" t="s">
+      <c r="C94" s="40" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B95" s="40" t="s">
+      <c r="B95" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="C95" s="40"/>
+      <c r="C95" s="39"/>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B96" s="41" t="s">
+      <c r="B96" s="40" t="s">
         <v>178</v>
       </c>
-      <c r="C96" s="41" t="s">
+      <c r="C96" s="40" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B97" s="41" t="s">
+      <c r="B97" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="C97" s="41" t="s">
+      <c r="C97" s="40" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B98" s="41" t="s">
+      <c r="B98" s="40" t="s">
         <v>182</v>
       </c>
-      <c r="C98" s="41" t="s">
+      <c r="C98" s="40" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B99" s="41" t="s">
+      <c r="B99" s="40" t="s">
         <v>184</v>
       </c>
-      <c r="C99" s="41" t="s">
+      <c r="C99" s="40" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B100" s="41" t="s">
+      <c r="B100" s="40" t="s">
         <v>186</v>
       </c>
-      <c r="C100" s="41" t="s">
+      <c r="C100" s="40" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B101" s="40" t="s">
+      <c r="B101" s="39" t="s">
         <v>188</v>
       </c>
-      <c r="C101" s="40"/>
+      <c r="C101" s="39"/>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B102" s="41" t="s">
+      <c r="B102" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C102" s="41" t="s">
+      <c r="C102" s="40" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B103" s="41" t="s">
+      <c r="B103" s="40" t="s">
         <v>191</v>
       </c>
-      <c r="C103" s="41" t="s">
+      <c r="C103" s="40" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B104" s="41" t="s">
+      <c r="B104" s="40" t="s">
         <v>193</v>
       </c>
-      <c r="C104" s="41" t="s">
+      <c r="C104" s="40" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B105" s="42" t="s">
+      <c r="B105" s="41" t="s">
         <v>195</v>
       </c>
-      <c r="C105" s="43"/>
+      <c r="C105" s="42"/>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B106" s="40" t="s">
+      <c r="B106" s="39" t="s">
         <v>196</v>
       </c>
-      <c r="C106" s="40"/>
+      <c r="C106" s="39"/>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B107" s="41" t="s">
+      <c r="B107" s="40" t="s">
         <v>197</v>
       </c>
-      <c r="C107" s="41" t="s">
+      <c r="C107" s="40" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B108" s="41" t="s">
+      <c r="B108" s="40" t="s">
         <v>199</v>
       </c>
-      <c r="C108" s="41" t="s">
+      <c r="C108" s="40" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B109" s="41" t="s">
+      <c r="B109" s="40" t="s">
         <v>201</v>
       </c>
-      <c r="C109" s="41" t="s">
+      <c r="C109" s="40" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B110" s="41" t="s">
+      <c r="B110" s="40" t="s">
         <v>203</v>
       </c>
-      <c r="C110" s="41" t="s">
+      <c r="C110" s="40" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B111" s="41" t="s">
+      <c r="B111" s="40" t="s">
         <v>205</v>
       </c>
-      <c r="C111" s="41" t="s">
+      <c r="C111" s="40" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B112" s="41" t="s">
+      <c r="B112" s="40" t="s">
         <v>207</v>
       </c>
-      <c r="C112" s="41" t="s">
+      <c r="C112" s="40" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B113" s="41" t="s">
+      <c r="B113" s="40" t="s">
         <v>209</v>
       </c>
-      <c r="C113" s="41" t="s">
+      <c r="C113" s="40" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B114" s="40" t="s">
+      <c r="B114" s="39" t="s">
         <v>211</v>
       </c>
-      <c r="C114" s="40"/>
+      <c r="C114" s="39"/>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B115" s="41" t="s">
+      <c r="B115" s="40" t="s">
         <v>212</v>
       </c>
-      <c r="C115" s="41" t="s">
+      <c r="C115" s="40" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B116" s="41" t="s">
+      <c r="B116" s="40" t="s">
         <v>214</v>
       </c>
-      <c r="C116" s="41" t="s">
+      <c r="C116" s="40" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B117" s="41" t="s">
+      <c r="B117" s="40" t="s">
         <v>216</v>
       </c>
-      <c r="C117" s="41" t="s">
+      <c r="C117" s="40" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B118" s="41" t="s">
+      <c r="B118" s="40" t="s">
         <v>218</v>
       </c>
-      <c r="C118" s="41" t="s">
+      <c r="C118" s="40" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B119" s="41" t="s">
+      <c r="B119" s="40" t="s">
         <v>220</v>
       </c>
-      <c r="C119" s="41" t="s">
+      <c r="C119" s="40" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B120" s="41" t="s">
+      <c r="B120" s="40" t="s">
         <v>222</v>
       </c>
-      <c r="C120" s="41" t="s">
+      <c r="C120" s="40" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B121" s="41" t="s">
+      <c r="B121" s="40" t="s">
         <v>224</v>
       </c>
-      <c r="C121" s="41" t="s">
+      <c r="C121" s="40" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B122" s="40" t="s">
+      <c r="B122" s="39" t="s">
         <v>226</v>
       </c>
-      <c r="C122" s="40"/>
+      <c r="C122" s="39"/>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B123" s="41" t="s">
+      <c r="B123" s="40" t="s">
         <v>227</v>
       </c>
-      <c r="C123" s="41" t="s">
+      <c r="C123" s="40" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B124" s="41" t="s">
+      <c r="B124" s="40" t="s">
         <v>229</v>
       </c>
-      <c r="C124" s="41" t="s">
+      <c r="C124" s="40" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B125" s="41" t="s">
+      <c r="B125" s="40" t="s">
         <v>231</v>
       </c>
-      <c r="C125" s="41" t="s">
+      <c r="C125" s="40" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B126" s="41" t="s">
+      <c r="B126" s="40" t="s">
         <v>233</v>
       </c>
-      <c r="C126" s="41" t="s">
+      <c r="C126" s="40" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B127" s="41" t="s">
+      <c r="B127" s="40" t="s">
         <v>235</v>
       </c>
-      <c r="C127" s="41" t="s">
+      <c r="C127" s="40" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B128" s="41" t="s">
+      <c r="B128" s="40" t="s">
         <v>237</v>
       </c>
-      <c r="C128" s="41" t="s">
+      <c r="C128" s="40" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B129" s="41" t="s">
+      <c r="B129" s="40" t="s">
         <v>239</v>
       </c>
-      <c r="C129" s="41" t="s">
+      <c r="C129" s="40" t="s">
         <v>240</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modify the unit of new vehicle sales in 2020 (divide by 1000)
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_NCAP_2020.xlsx
+++ b/SuppXLS/Scen_TRA_NCAP_2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009D73EB-43FC-4089-B9E4-CFE3954EBE33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10EF47D-8334-4280-9283-A986B9641EAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -870,7 +870,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1411,7 +1411,7 @@
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1462,8 +1462,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1490,6 +1488,9 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="273">
     <cellStyle name="20% - Accent5 2" xfId="13" xr:uid="{10C4E126-2686-43C7-AD29-7BC90D313B29}"/>
@@ -3080,7 +3081,7 @@
   <dimension ref="A1:AH24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3095,7 +3096,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" s="19" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>241</v>
       </c>
     </row>
@@ -3257,113 +3258,113 @@
       <c r="E7">
         <v>2020</v>
       </c>
-      <c r="F7" s="32">
-        <f>'New vehicle sales'!C6</f>
-        <v>38233</v>
+      <c r="F7" s="42">
+        <f>'New vehicle sales'!C6/1000</f>
+        <v>38.232999999999997</v>
       </c>
       <c r="G7" s="24">
         <f>$F$7*'New vehicle sales'!D43</f>
-        <v>457.10685960227732</v>
+        <v>0.45710685960227732</v>
       </c>
       <c r="H7" s="24">
         <f>$F$7*'New vehicle sales'!E43</f>
-        <v>10817.941425680916</v>
+        <v>10.817941425680914</v>
       </c>
       <c r="I7" s="24">
         <f>$F$7*'New vehicle sales'!F43</f>
-        <v>1786.4839578610467</v>
+        <v>1.7864839578610465</v>
       </c>
       <c r="J7" s="24">
         <f>$F$7*'New vehicle sales'!G43</f>
-        <v>796.73343448417734</v>
+        <v>0.79673343448417733</v>
       </c>
       <c r="K7" s="24">
         <f>$F$7*'New vehicle sales'!H43</f>
-        <v>680.03196247688618</v>
+        <v>0.68003196247688613</v>
       </c>
       <c r="L7" s="24">
         <f>$F$7*'New vehicle sales'!I43</f>
-        <v>328.16919610278723</v>
+        <v>0.32816919610278722</v>
       </c>
       <c r="M7" s="24">
         <f>$F$7*'New vehicle sales'!J43</f>
-        <v>1034.8092547772767</v>
+        <v>1.0348092547772767</v>
       </c>
       <c r="N7" s="24">
         <f>$F$7*'New vehicle sales'!K43</f>
-        <v>1566.0076990842861</v>
+        <v>1.5660076990842859</v>
       </c>
       <c r="O7" s="24">
         <f>$F$7*'New vehicle sales'!L43</f>
-        <v>625.94863840113021</v>
+        <v>0.62594863840113013</v>
       </c>
       <c r="P7" s="24">
         <f>$F$7*'New vehicle sales'!M43</f>
-        <v>712.73406742946247</v>
+        <v>0.71273406742946244</v>
       </c>
       <c r="Q7" s="24">
         <f>$F$7*'New vehicle sales'!N43</f>
-        <v>1202.1174951410835</v>
+        <v>1.2021174951410833</v>
       </c>
       <c r="R7" s="24">
         <f>$F$7*'New vehicle sales'!O43</f>
-        <v>1143.5299037246953</v>
+        <v>1.1435299037246951</v>
       </c>
       <c r="S7" s="24">
         <f>$F$7*'New vehicle sales'!P43</f>
-        <v>953.98134155420121</v>
+        <v>0.95398134155420122</v>
       </c>
       <c r="T7" s="24">
         <f>$F$7*'New vehicle sales'!Q43</f>
-        <v>4358.6855662644757</v>
+        <v>4.3586855662644748</v>
       </c>
       <c r="U7" s="24">
         <f>$F$7*'New vehicle sales'!R43</f>
-        <v>1185.9390661012012</v>
+        <v>1.185939066101201</v>
       </c>
       <c r="V7" s="24">
         <f>$F$7*'New vehicle sales'!S43</f>
-        <v>1564.843494513178</v>
+        <v>1.5648434945131779</v>
       </c>
       <c r="W7" s="24">
         <f>$F$7*'New vehicle sales'!T43</f>
-        <v>1281.0505650622174</v>
+        <v>1.2810505650622175</v>
       </c>
       <c r="X7" s="24">
         <f>$F$7*'New vehicle sales'!U43</f>
-        <v>932.77676036594835</v>
+        <v>0.93277676036594825</v>
       </c>
       <c r="Y7" s="24">
         <f>$F$7*'New vehicle sales'!V43</f>
-        <v>2071.9469186967694</v>
+        <v>2.0719469186967694</v>
       </c>
       <c r="Z7" s="24">
         <f>$F$7*'New vehicle sales'!W43</f>
-        <v>257.28118121786298</v>
+        <v>0.25728118121786298</v>
       </c>
       <c r="AA7" s="24">
         <f>$F$7*'New vehicle sales'!X43</f>
-        <v>1047.8403169766461</v>
+        <v>1.0478403169766459</v>
       </c>
       <c r="AB7" s="24">
         <f>$F$7*'New vehicle sales'!Y43</f>
-        <v>518.22358508693503</v>
+        <v>0.518223585086935</v>
       </c>
       <c r="AC7" s="24">
         <f>$F$7*'New vehicle sales'!Z43</f>
-        <v>526.18032115568121</v>
+        <v>0.52618032115568125</v>
       </c>
       <c r="AD7" s="24">
         <f>$F$7*'New vehicle sales'!AA43</f>
-        <v>611.61687868093657</v>
+        <v>0.6116168786809365</v>
       </c>
       <c r="AE7" s="24">
         <f>$F$7*'New vehicle sales'!AB43</f>
-        <v>1278.1520971300099</v>
+        <v>1.2781520971300098</v>
       </c>
       <c r="AF7" s="24">
         <f>$F$7*'New vehicle sales'!AC43</f>
-        <v>492.86801242790341</v>
+        <v>0.49286801242790335</v>
       </c>
       <c r="AG7" t="str">
         <f>'New vehicle sales'!B57</f>
@@ -3383,113 +3384,113 @@
       <c r="E8" s="19">
         <v>2020</v>
       </c>
-      <c r="F8" s="32">
-        <f>'New vehicle sales'!C7</f>
-        <v>32600</v>
+      <c r="F8" s="42">
+        <f>'New vehicle sales'!C7/1000</f>
+        <v>32.6</v>
       </c>
       <c r="G8" s="24">
         <f>$F$8*'New vehicle sales'!D43</f>
-        <v>389.75972649371596</v>
+        <v>0.38975972649371593</v>
       </c>
       <c r="H8" s="24">
         <f>$F$8*'New vehicle sales'!E43</f>
-        <v>9224.0967352077478</v>
+        <v>9.2240967352077483</v>
       </c>
       <c r="I8" s="24">
         <f>$F$8*'New vehicle sales'!F43</f>
-        <v>1523.2751033471118</v>
+        <v>1.5232751033471117</v>
       </c>
       <c r="J8" s="24">
         <f>$F$8*'New vehicle sales'!G43</f>
-        <v>679.34794455533654</v>
+        <v>0.67934794455533654</v>
       </c>
       <c r="K8" s="24">
         <f>$F$8*'New vehicle sales'!H43</f>
-        <v>579.8405036682052</v>
+        <v>0.57984050366820528</v>
       </c>
       <c r="L8" s="24">
         <f>$F$8*'New vehicle sales'!I43</f>
-        <v>279.81889448776877</v>
+        <v>0.27981889448776881</v>
       </c>
       <c r="M8" s="24">
         <f>$F$8*'New vehicle sales'!J43</f>
-        <v>882.34723159938324</v>
+        <v>0.88234723159938333</v>
       </c>
       <c r="N8" s="24">
         <f>$F$8*'New vehicle sales'!K43</f>
-        <v>1335.2823736078185</v>
+        <v>1.3352823736078185</v>
       </c>
       <c r="O8" s="24">
         <f>$F$8*'New vehicle sales'!L43</f>
-        <v>533.72546260761237</v>
+        <v>0.53372546260761244</v>
       </c>
       <c r="P8" s="24">
         <f>$F$8*'New vehicle sales'!M43</f>
-        <v>607.72449449952865</v>
+        <v>0.60772449449952859</v>
       </c>
       <c r="Q8" s="24">
         <f>$F$8*'New vehicle sales'!N43</f>
-        <v>1025.0053707948455</v>
+        <v>1.0250053707948454</v>
       </c>
       <c r="R8" s="24">
         <f>$F$8*'New vehicle sales'!O43</f>
-        <v>975.04969166492469</v>
+        <v>0.97504969166492472</v>
       </c>
       <c r="S8" s="24">
         <f>$F$8*'New vehicle sales'!P43</f>
-        <v>813.42797412358334</v>
+        <v>0.81342797412358336</v>
       </c>
       <c r="T8" s="24">
         <f>$F$8*'New vehicle sales'!Q43</f>
-        <v>3716.5053608197604</v>
+        <v>3.7165053608197605</v>
       </c>
       <c r="U8" s="24">
         <f>$F$8*'New vehicle sales'!R43</f>
-        <v>1011.2105656082222</v>
+        <v>1.0112105656082222</v>
       </c>
       <c r="V8" s="24">
         <f>$F$8*'New vehicle sales'!S43</f>
-        <v>1334.289695318955</v>
+        <v>1.3342896953189549</v>
       </c>
       <c r="W8" s="24">
         <f>$F$8*'New vehicle sales'!T43</f>
-        <v>1092.3089587798052</v>
+        <v>1.0923089587798052</v>
       </c>
       <c r="X8" s="24">
         <f>$F$8*'New vehicle sales'!U43</f>
-        <v>795.3475371519346</v>
+        <v>0.79534753715193462</v>
       </c>
       <c r="Y8" s="24">
         <f>$F$8*'New vehicle sales'!V43</f>
-        <v>1766.6798197764938</v>
+        <v>1.7666798197764939</v>
       </c>
       <c r="Z8" s="24">
         <f>$F$8*'New vehicle sales'!W43</f>
-        <v>219.37505578171562</v>
+        <v>0.21937505578171562</v>
       </c>
       <c r="AA8" s="24">
         <f>$F$8*'New vehicle sales'!X43</f>
-        <v>893.45838237749228</v>
+        <v>0.89345838237749231</v>
       </c>
       <c r="AB8" s="24">
         <f>$F$8*'New vehicle sales'!Y43</f>
-        <v>441.87191363047845</v>
+        <v>0.44187191363047851</v>
       </c>
       <c r="AC8" s="24">
         <f>$F$8*'New vehicle sales'!Z43</f>
-        <v>448.65635628057458</v>
+        <v>0.44865635628057465</v>
       </c>
       <c r="AD8" s="24">
         <f>$F$8*'New vehicle sales'!AA43</f>
-        <v>521.5052505688418</v>
+        <v>0.52150525056884189</v>
       </c>
       <c r="AE8" s="24">
         <f>$F$8*'New vehicle sales'!AB43</f>
-        <v>1089.8375321433925</v>
+        <v>1.0898375321433926</v>
       </c>
       <c r="AF8" s="24">
         <f>$F$8*'New vehicle sales'!AC43</f>
-        <v>420.25206510474334</v>
+        <v>0.42025206510474333</v>
       </c>
       <c r="AG8" t="str">
         <f>'New vehicle sales'!B56</f>
@@ -3509,113 +3510,113 @@
       <c r="E9" s="19">
         <v>2020</v>
       </c>
-      <c r="F9" s="32">
-        <f>'New vehicle sales'!C8</f>
-        <v>10474</v>
+      <c r="F9" s="42">
+        <f>'New vehicle sales'!C8/1000</f>
+        <v>10.474</v>
       </c>
       <c r="G9" s="24">
         <f>$F$9*'New vehicle sales'!D43</f>
-        <v>125.22525691089511</v>
+        <v>0.12522525691089512</v>
       </c>
       <c r="H9" s="24">
         <f>$F$9*'New vehicle sales'!E43</f>
-        <v>2963.5947608762563</v>
+        <v>2.9635947608762563</v>
       </c>
       <c r="I9" s="24">
         <f>$F$9*'New vehicle sales'!F43</f>
-        <v>489.41053473796467</v>
+        <v>0.4894105347379647</v>
       </c>
       <c r="J9" s="24">
         <f>$F$9*'New vehicle sales'!G43</f>
-        <v>218.26657580590782</v>
+        <v>0.21826657580590783</v>
       </c>
       <c r="K9" s="24">
         <f>$F$9*'New vehicle sales'!H43</f>
-        <v>186.2959949515577</v>
+        <v>0.18629599495155771</v>
       </c>
       <c r="L9" s="24">
         <f>$F$9*'New vehicle sales'!I43</f>
-        <v>89.90254910628498</v>
+        <v>8.9902549106284979E-2</v>
       </c>
       <c r="M9" s="24">
         <f>$F$9*'New vehicle sales'!J43</f>
-        <v>283.48788048380186</v>
+        <v>0.28348788048380186</v>
       </c>
       <c r="N9" s="24">
         <f>$F$9*'New vehicle sales'!K43</f>
-        <v>429.01066199902738</v>
+        <v>0.42901066199902738</v>
       </c>
       <c r="O9" s="24">
         <f>$F$9*'New vehicle sales'!L43</f>
-        <v>171.47976979607768</v>
+        <v>0.17147976979607768</v>
       </c>
       <c r="P9" s="24">
         <f>$F$9*'New vehicle sales'!M43</f>
-        <v>195.25479617754795</v>
+        <v>0.19525479617754793</v>
       </c>
       <c r="Q9" s="24">
         <f>$F$9*'New vehicle sales'!N43</f>
-        <v>329.32227772101874</v>
+        <v>0.32932227772101874</v>
       </c>
       <c r="R9" s="24">
         <f>$F$9*'New vehicle sales'!O43</f>
-        <v>313.27210032203743</v>
+        <v>0.31327210032203745</v>
       </c>
       <c r="S9" s="24">
         <f>$F$9*'New vehicle sales'!P43</f>
-        <v>261.34492641013532</v>
+        <v>0.26134492641013535</v>
       </c>
       <c r="T9" s="24">
         <f>$F$9*'New vehicle sales'!Q43</f>
-        <v>1194.0698512032568</v>
+        <v>1.1940698512032568</v>
       </c>
       <c r="U9" s="24">
         <f>$F$9*'New vehicle sales'!R43</f>
-        <v>324.89016761289935</v>
+        <v>0.32489016761289935</v>
       </c>
       <c r="V9" s="24">
         <f>$F$9*'New vehicle sales'!S43</f>
-        <v>428.6917260359121</v>
+        <v>0.4286917260359121</v>
       </c>
       <c r="W9" s="24">
         <f>$F$9*'New vehicle sales'!T43</f>
-        <v>350.94613602023554</v>
+        <v>0.35094613602023556</v>
       </c>
       <c r="X9" s="24">
         <f>$F$9*'New vehicle sales'!U43</f>
-        <v>255.53589276470439</v>
+        <v>0.2555358927647044</v>
       </c>
       <c r="Y9" s="24">
         <f>$F$9*'New vehicle sales'!V43</f>
-        <v>567.61363289383428</v>
+        <v>0.56761363289383426</v>
       </c>
       <c r="Z9" s="24">
         <f>$F$9*'New vehicle sales'!W43</f>
-        <v>70.482648290113175</v>
+        <v>7.0482648290113165E-2</v>
       </c>
       <c r="AA9" s="24">
         <f>$F$9*'New vehicle sales'!X43</f>
-        <v>287.05776371232679</v>
+        <v>0.28705776371232683</v>
       </c>
       <c r="AB9" s="24">
         <f>$F$9*'New vehicle sales'!Y43</f>
-        <v>141.96829519526477</v>
+        <v>0.14196829519526477</v>
       </c>
       <c r="AC9" s="24">
         <f>$F$9*'New vehicle sales'!Z43</f>
-        <v>144.14805753628033</v>
+        <v>0.14414805753628032</v>
       </c>
       <c r="AD9" s="24">
         <f>$F$9*'New vehicle sales'!AA43</f>
-        <v>167.55355811221011</v>
+        <v>0.16755355811221012</v>
       </c>
       <c r="AE9" s="24">
         <f>$F$9*'New vehicle sales'!AB43</f>
-        <v>350.15209544999669</v>
+        <v>0.3501520954499967</v>
       </c>
       <c r="AF9" s="24">
         <f>$F$9*'New vehicle sales'!AC43</f>
-        <v>135.02208987445036</v>
+        <v>0.13502208987445036</v>
       </c>
       <c r="AG9" t="str">
         <f>'New vehicle sales'!B62</f>
@@ -3635,113 +3636,113 @@
       <c r="E10" s="19">
         <v>2020</v>
       </c>
-      <c r="F10" s="32">
-        <f>'New vehicle sales'!C9</f>
-        <v>4013</v>
+      <c r="F10" s="42">
+        <f>'New vehicle sales'!C9/1000</f>
+        <v>4.0129999999999999</v>
       </c>
       <c r="G10" s="24">
         <f>$F$10*'New vehicle sales'!D43</f>
-        <v>47.978704982186564</v>
+        <v>4.7978704982186565E-2</v>
       </c>
       <c r="H10" s="24">
         <f>$F$10*'New vehicle sales'!E43</f>
-        <v>1135.469331238917</v>
+        <v>1.135469331238917</v>
       </c>
       <c r="I10" s="24">
         <f>$F$10*'New vehicle sales'!F43</f>
-        <v>187.51236164821961</v>
+        <v>0.18751236164821961</v>
       </c>
       <c r="J10" s="24">
         <f>$F$10*'New vehicle sales'!G43</f>
-        <v>83.626481641121643</v>
+        <v>8.3626481641121644E-2</v>
       </c>
       <c r="K10" s="24">
         <f>$F$10*'New vehicle sales'!H43</f>
-        <v>71.377298810445012</v>
+        <v>7.1377298810445008E-2</v>
       </c>
       <c r="L10" s="24">
         <f>$F$10*'New vehicle sales'!I43</f>
-        <v>34.445190907344056</v>
+        <v>3.4445190907344055E-2</v>
       </c>
       <c r="M10" s="24">
         <f>$F$10*'New vehicle sales'!J43</f>
-        <v>108.61532025792408</v>
+        <v>0.10861532025792409</v>
       </c>
       <c r="N10" s="24">
         <f>$F$10*'New vehicle sales'!K43</f>
-        <v>164.37080261620173</v>
+        <v>0.16437080261620171</v>
       </c>
       <c r="O10" s="24">
         <f>$F$10*'New vehicle sales'!L43</f>
-        <v>65.700622130194731</v>
+        <v>6.570062213019473E-2</v>
       </c>
       <c r="P10" s="24">
         <f>$F$10*'New vehicle sales'!M43</f>
-        <v>74.809766761552396</v>
+        <v>7.4809766761552404E-2</v>
       </c>
       <c r="Q10" s="24">
         <f>$F$10*'New vehicle sales'!N43</f>
-        <v>126.17627463189308</v>
+        <v>0.12617627463189307</v>
       </c>
       <c r="R10" s="24">
         <f>$F$10*'New vehicle sales'!O43</f>
-        <v>120.02682247396757</v>
+        <v>0.12002682247396756</v>
       </c>
       <c r="S10" s="24">
         <f>$F$10*'New vehicle sales'!P43</f>
-        <v>100.13148650791227</v>
+        <v>0.10013148650791226</v>
       </c>
       <c r="T10" s="24">
         <f>$F$10*'New vehicle sales'!Q43</f>
-        <v>457.49496972299687</v>
+        <v>0.45749496972299686</v>
       </c>
       <c r="U10" s="24">
         <f>$F$10*'New vehicle sales'!R43</f>
-        <v>124.47815950263177</v>
+        <v>0.12447815950263176</v>
       </c>
       <c r="V10" s="24">
         <f>$F$10*'New vehicle sales'!S43</f>
-        <v>164.24860574585784</v>
+        <v>0.16424860574585784</v>
       </c>
       <c r="W10" s="24">
         <f>$F$10*'New vehicle sales'!T43</f>
-        <v>134.4612224412073</v>
+        <v>0.13446122244120728</v>
       </c>
       <c r="X10" s="24">
         <f>$F$10*'New vehicle sales'!U43</f>
-        <v>97.905817993580172</v>
+        <v>9.7905817993580169E-2</v>
       </c>
       <c r="Y10" s="24">
         <f>$F$10*'New vehicle sales'!V43</f>
-        <v>217.47503425653588</v>
+        <v>0.21747503425653589</v>
       </c>
       <c r="Z10" s="24">
         <f>$F$10*'New vehicle sales'!W43</f>
-        <v>27.004665608957815</v>
+        <v>2.7004665608957815E-2</v>
       </c>
       <c r="AA10" s="24">
         <f>$F$10*'New vehicle sales'!X43</f>
-        <v>109.98308246873854</v>
+        <v>0.10998308246873854</v>
       </c>
       <c r="AB10" s="24">
         <f>$F$10*'New vehicle sales'!Y43</f>
-        <v>54.39361930672117</v>
+        <v>5.4393619306721167E-2</v>
       </c>
       <c r="AC10" s="24">
         <f>$F$10*'New vehicle sales'!Z43</f>
-        <v>55.228771710243741</v>
+        <v>5.5228771710243735E-2</v>
       </c>
       <c r="AD10" s="24">
         <f>$F$10*'New vehicle sales'!AA43</f>
-        <v>64.196336519409883</v>
+        <v>6.4196336519409883E-2</v>
       </c>
       <c r="AE10" s="24">
         <f>$F$10*'New vehicle sales'!AB43</f>
-        <v>134.15699437090288</v>
+        <v>0.13415699437090289</v>
       </c>
       <c r="AF10" s="24">
         <f>$F$10*'New vehicle sales'!AC43</f>
-        <v>51.732255744335426</v>
+        <v>5.1732255744335424E-2</v>
       </c>
       <c r="AG10" t="str">
         <f>'New vehicle sales'!B70</f>
@@ -3761,113 +3762,113 @@
       <c r="E11" s="19">
         <v>2020</v>
       </c>
-      <c r="F11" s="32">
-        <f>'New vehicle sales'!C10</f>
-        <v>2459</v>
+      <c r="F11" s="42">
+        <f>'New vehicle sales'!C10/1000</f>
+        <v>2.4590000000000001</v>
       </c>
       <c r="G11" s="24">
         <f>$F$11*'New vehicle sales'!D43</f>
-        <v>29.399360964664034</v>
+        <v>2.9399360964664036E-2</v>
       </c>
       <c r="H11" s="24">
         <f>$F$11*'New vehicle sales'!E43</f>
-        <v>695.76852367717345</v>
+        <v>0.69576852367717346</v>
       </c>
       <c r="I11" s="24">
         <f>$F$11*'New vehicle sales'!F43</f>
-        <v>114.89979997332968</v>
+        <v>0.11489979997332969</v>
       </c>
       <c r="J11" s="24">
         <f>$F$11*'New vehicle sales'!G43</f>
-        <v>51.24284035771695</v>
+        <v>5.1242840357716951E-2</v>
       </c>
       <c r="K11" s="24">
         <f>$F$11*'New vehicle sales'!H43</f>
-        <v>43.737049034359401</v>
+        <v>4.3737049034359404E-2</v>
       </c>
       <c r="L11" s="24">
         <f>$F$11*'New vehicle sales'!I43</f>
-        <v>21.106584709982315</v>
+        <v>2.1106584709982317E-2</v>
       </c>
       <c r="M11" s="24">
         <f>$F$11*'New vehicle sales'!J43</f>
-        <v>66.554964493953477</v>
+        <v>6.6554964493953483E-2</v>
       </c>
       <c r="N11" s="24">
         <f>$F$11*'New vehicle sales'!K43</f>
-        <v>100.71961216876153</v>
+        <v>0.10071961216876153</v>
       </c>
       <c r="O11" s="24">
         <f>$F$11*'New vehicle sales'!L43</f>
-        <v>40.2586169494515</v>
+        <v>4.0258616949451501E-2</v>
       </c>
       <c r="P11" s="24">
         <f>$F$11*'New vehicle sales'!M43</f>
-        <v>45.840323066697572</v>
+        <v>4.5840323066697573E-2</v>
       </c>
       <c r="Q11" s="24">
         <f>$F$11*'New vehicle sales'!N43</f>
-        <v>77.31558916516947</v>
+        <v>7.7315589165169479E-2</v>
       </c>
       <c r="R11" s="24">
         <f>$F$11*'New vehicle sales'!O43</f>
-        <v>73.547459871289874</v>
+        <v>7.3547459871289869E-2</v>
       </c>
       <c r="S11" s="24">
         <f>$F$11*'New vehicle sales'!P43</f>
-        <v>61.356422956131638</v>
+        <v>6.135642295613164E-2</v>
       </c>
       <c r="T11" s="24">
         <f>$F$11*'New vehicle sales'!Q43</f>
-        <v>280.33394730845981</v>
+        <v>0.28033394730845984</v>
       </c>
       <c r="U11" s="24">
         <f>$F$11*'New vehicle sales'!R43</f>
-        <v>76.27505462670608</v>
+        <v>7.6275054626706085E-2</v>
       </c>
       <c r="V11" s="24">
         <f>$F$11*'New vehicle sales'!S43</f>
-        <v>100.64473499353711</v>
+        <v>0.10064473499353713</v>
       </c>
       <c r="W11" s="24">
         <f>$F$11*'New vehicle sales'!T43</f>
-        <v>82.392261645384693</v>
+        <v>8.2392261645384685E-2</v>
       </c>
       <c r="X11" s="24">
         <f>$F$11*'New vehicle sales'!U43</f>
-        <v>59.992625578423535</v>
+        <v>5.9992625578423532E-2</v>
       </c>
       <c r="Y11" s="24">
         <f>$F$11*'New vehicle sales'!V43</f>
-        <v>133.25968333835579</v>
+        <v>0.13325968333835578</v>
       </c>
       <c r="Z11" s="24">
         <f>$F$11*'New vehicle sales'!W43</f>
-        <v>16.547339330283396</v>
+        <v>1.6547339330283396E-2</v>
       </c>
       <c r="AA11" s="24">
         <f>$F$11*'New vehicle sales'!X43</f>
-        <v>67.393072462155018</v>
+        <v>6.7393072462155021E-2</v>
       </c>
       <c r="AB11" s="24">
         <f>$F$11*'New vehicle sales'!Y43</f>
-        <v>33.330154466789772</v>
+        <v>3.3330154466789774E-2</v>
       </c>
       <c r="AC11" s="24">
         <f>$F$11*'New vehicle sales'!Z43</f>
-        <v>33.841901229875248</v>
+        <v>3.3841901229875244E-2</v>
       </c>
       <c r="AD11" s="24">
         <f>$F$11*'New vehicle sales'!AA43</f>
-        <v>39.336853102723374</v>
+        <v>3.9336853102723376E-2</v>
       </c>
       <c r="AE11" s="24">
         <f>$F$11*'New vehicle sales'!AB43</f>
-        <v>82.205843298791478</v>
+        <v>8.2205843298791478E-2</v>
       </c>
       <c r="AF11" s="24">
         <f>$F$11*'New vehicle sales'!AC43</f>
-        <v>31.699381229833246</v>
+        <v>3.1699381229833248E-2</v>
       </c>
       <c r="AG11" t="str">
         <f>'New vehicle sales'!B66</f>
@@ -3887,113 +3888,113 @@
       <c r="E12" s="19">
         <v>2020</v>
       </c>
-      <c r="F12" s="32">
-        <f>'New vehicle sales'!C11</f>
-        <v>512</v>
+      <c r="F12" s="42">
+        <f>'New vehicle sales'!C11/1000</f>
+        <v>0.51200000000000001</v>
       </c>
       <c r="G12" s="24">
         <f>$F$12*'New vehicle sales'!D43</f>
-        <v>6.1213797535209373</v>
+        <v>6.1213797535209372E-3</v>
       </c>
       <c r="H12" s="24">
         <f>$F$12*'New vehicle sales'!E43</f>
-        <v>144.86924933823212</v>
+        <v>0.14486924933823211</v>
       </c>
       <c r="I12" s="24">
         <f>$F$12*'New vehicle sales'!F43</f>
-        <v>23.923829843979178</v>
+        <v>2.3923829843979179E-2</v>
       </c>
       <c r="J12" s="24">
         <f>$F$12*'New vehicle sales'!G43</f>
-        <v>10.669513730439641</v>
+        <v>1.0669513730439641E-2</v>
       </c>
       <c r="K12" s="24">
         <f>$F$12*'New vehicle sales'!H43</f>
-        <v>9.1066974809239589</v>
+        <v>9.106697480923959E-3</v>
       </c>
       <c r="L12" s="24">
         <f>$F$12*'New vehicle sales'!I43</f>
-        <v>4.3947016557588228</v>
+        <v>4.3947016557588231E-3</v>
       </c>
       <c r="M12" s="24">
         <f>$F$12*'New vehicle sales'!J43</f>
-        <v>13.857723391990314</v>
+        <v>1.3857723391990314E-2</v>
       </c>
       <c r="N12" s="24">
         <f>$F$12*'New vehicle sales'!K43</f>
-        <v>20.971305990405003</v>
+        <v>2.0971305990405004E-2</v>
       </c>
       <c r="O12" s="24">
         <f>$F$12*'New vehicle sales'!L43</f>
-        <v>8.3824367133465501</v>
+        <v>8.3824367133465503E-3</v>
       </c>
       <c r="P12" s="24">
         <f>$F$12*'New vehicle sales'!M43</f>
-        <v>9.5446300976613081</v>
+        <v>9.544630097661308E-3</v>
       </c>
       <c r="Q12" s="24">
         <f>$F$12*'New vehicle sales'!N43</f>
-        <v>16.098243860336222</v>
+        <v>1.6098243860336221E-2</v>
       </c>
       <c r="R12" s="24">
         <f>$F$12*'New vehicle sales'!O43</f>
-        <v>15.313663869093295</v>
+        <v>1.5313663869093296E-2</v>
       </c>
       <c r="S12" s="24">
         <f>$F$12*'New vehicle sales'!P43</f>
-        <v>12.775310513842781</v>
+        <v>1.2775310513842781E-2</v>
       </c>
       <c r="T12" s="24">
         <f>$F$12*'New vehicle sales'!Q43</f>
-        <v>58.369654746617094</v>
+        <v>5.8369654746617095E-2</v>
       </c>
       <c r="U12" s="24">
         <f>$F$12*'New vehicle sales'!R43</f>
-        <v>15.881589251270238</v>
+        <v>1.5881589251270239E-2</v>
       </c>
       <c r="V12" s="24">
         <f>$F$12*'New vehicle sales'!S43</f>
-        <v>20.955715460224077</v>
+        <v>2.0955715460224077E-2</v>
       </c>
       <c r="W12" s="24">
         <f>$F$12*'New vehicle sales'!T43</f>
-        <v>17.155281806603075</v>
+        <v>1.7155281806603074E-2</v>
       </c>
       <c r="X12" s="24">
         <f>$F$12*'New vehicle sales'!U43</f>
-        <v>12.49134782275431</v>
+        <v>1.2491347822754311E-2</v>
       </c>
       <c r="Y12" s="24">
         <f>$F$12*'New vehicle sales'!V43</f>
-        <v>27.746627844342481</v>
+        <v>2.7746627844342481E-2</v>
       </c>
       <c r="Z12" s="24">
         <f>$F$12*'New vehicle sales'!W43</f>
-        <v>3.4453996490870673</v>
+        <v>3.4453996490870675E-3</v>
       </c>
       <c r="AA12" s="24">
         <f>$F$12*'New vehicle sales'!X43</f>
-        <v>14.032229809118897</v>
+        <v>1.4032229809118897E-2</v>
       </c>
       <c r="AB12" s="24">
         <f>$F$12*'New vehicle sales'!Y43</f>
-        <v>6.9398288275707047</v>
+        <v>6.939828827570705E-3</v>
       </c>
       <c r="AC12" s="24">
         <f>$F$12*'New vehicle sales'!Z43</f>
-        <v>7.0463820372900061</v>
+        <v>7.0463820372900065E-3</v>
       </c>
       <c r="AD12" s="24">
         <f>$F$12*'New vehicle sales'!AA43</f>
-        <v>8.1905119107744486</v>
+        <v>8.1905119107744482E-3</v>
       </c>
       <c r="AE12" s="24">
         <f>$F$12*'New vehicle sales'!AB43</f>
-        <v>17.116466762497453</v>
+        <v>1.7116466762497454E-2</v>
       </c>
       <c r="AF12" s="24">
         <f>$F$12*'New vehicle sales'!AC43</f>
-        <v>6.600277832319895</v>
+        <v>6.6002778323198952E-3</v>
       </c>
       <c r="AG12" t="str">
         <f>'New vehicle sales'!B63</f>
@@ -4013,113 +4014,113 @@
       <c r="E13" s="19">
         <v>2020</v>
       </c>
-      <c r="F13" s="32">
-        <f>'New vehicle sales'!C12</f>
-        <v>33</v>
+      <c r="F13" s="42">
+        <f>'New vehicle sales'!C12/1000</f>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="G13" s="24">
         <f>$F$13*'New vehicle sales'!D43</f>
-        <v>0.39454205442615414</v>
+        <v>3.9454205442615418E-4</v>
       </c>
       <c r="H13" s="24">
         <f>$F$13*'New vehicle sales'!E43</f>
-        <v>9.3372758362532426</v>
+        <v>9.3372758362532428E-3</v>
       </c>
       <c r="I13" s="24">
         <f>$F$13*'New vehicle sales'!F43</f>
-        <v>1.5419655954127205</v>
+        <v>1.5419655954127206E-3</v>
       </c>
       <c r="J13" s="24">
         <f>$F$13*'New vehicle sales'!G43</f>
-        <v>0.6876835021572425</v>
+        <v>6.8768350215724257E-4</v>
       </c>
       <c r="K13" s="24">
         <f>$F$13*'New vehicle sales'!H43</f>
-        <v>0.58695511107517706</v>
+        <v>5.8695511107517706E-4</v>
       </c>
       <c r="L13" s="24">
         <f>$F$13*'New vehicle sales'!I43</f>
-        <v>0.28325225515633035</v>
+        <v>2.8325225515633037E-4</v>
       </c>
       <c r="M13" s="24">
         <f>$F$13*'New vehicle sales'!J43</f>
-        <v>0.89317357799937569</v>
+        <v>8.9317357799937572E-4</v>
       </c>
       <c r="N13" s="24">
         <f>$F$13*'New vehicle sales'!K43</f>
-        <v>1.3516662064128224</v>
+        <v>1.3516662064128224E-3</v>
       </c>
       <c r="O13" s="24">
         <f>$F$13*'New vehicle sales'!L43</f>
-        <v>0.54027424128991441</v>
+        <v>5.4027424128991436E-4</v>
       </c>
       <c r="P13" s="24">
         <f>$F$13*'New vehicle sales'!M43</f>
-        <v>0.61518123676332648</v>
+        <v>6.1518123676332652E-4</v>
       </c>
       <c r="Q13" s="24">
         <f>$F$13*'New vehicle sales'!N43</f>
-        <v>1.037582123810733</v>
+        <v>1.0375821238107332E-3</v>
       </c>
       <c r="R13" s="24">
         <f>$F$13*'New vehicle sales'!O43</f>
-        <v>0.98701349156265383</v>
+        <v>9.8701349156265377E-4</v>
       </c>
       <c r="S13" s="24">
         <f>$F$13*'New vehicle sales'!P43</f>
-        <v>0.82340868546252299</v>
+        <v>8.2340868546252298E-4</v>
       </c>
       <c r="T13" s="24">
         <f>$F$13*'New vehicle sales'!Q43</f>
-        <v>3.7621066535905547</v>
+        <v>3.7621066535905552E-3</v>
       </c>
       <c r="U13" s="24">
         <f>$F$13*'New vehicle sales'!R43</f>
-        <v>1.0236180572107771</v>
+        <v>1.0236180572107771E-3</v>
       </c>
       <c r="V13" s="24">
         <f>$F$13*'New vehicle sales'!S43</f>
-        <v>1.3506613480222549</v>
+        <v>1.3506613480222551E-3</v>
       </c>
       <c r="W13" s="24">
         <f>$F$13*'New vehicle sales'!T43</f>
-        <v>1.1057115226912138</v>
+        <v>1.1057115226912138E-3</v>
       </c>
       <c r="X13" s="24">
         <f>$F$13*'New vehicle sales'!U43</f>
-        <v>0.80510640263846145</v>
+        <v>8.051064026384614E-4</v>
       </c>
       <c r="Y13" s="24">
         <f>$F$13*'New vehicle sales'!V43</f>
-        <v>1.7883568727798864</v>
+        <v>1.7883568727798866E-3</v>
       </c>
       <c r="Z13" s="24">
         <f>$F$13*'New vehicle sales'!W43</f>
-        <v>0.22206677425756488</v>
+        <v>2.2206677425756489E-4</v>
       </c>
       <c r="AA13" s="24">
         <f>$F$13*'New vehicle sales'!X43</f>
-        <v>0.90442106191586646</v>
+        <v>9.0442106191586651E-4</v>
       </c>
       <c r="AB13" s="24">
         <f>$F$13*'New vehicle sales'!Y43</f>
-        <v>0.44729365490201806</v>
+        <v>4.4729365490201812E-4</v>
       </c>
       <c r="AC13" s="24">
         <f>$F$13*'New vehicle sales'!Z43</f>
-        <v>0.45416134224720744</v>
+        <v>4.5416134224720743E-4</v>
       </c>
       <c r="AD13" s="24">
         <f>$F$13*'New vehicle sales'!AA43</f>
-        <v>0.52790408799913435</v>
+        <v>5.2790408799913439E-4</v>
       </c>
       <c r="AE13" s="24">
         <f>$F$13*'New vehicle sales'!AB43</f>
-        <v>1.1032097718015936</v>
+        <v>1.1032097718015937E-3</v>
       </c>
       <c r="AF13" s="24">
         <f>$F$13*'New vehicle sales'!AC43</f>
-        <v>0.42540853216124325</v>
+        <v>4.2540853216124324E-4</v>
       </c>
       <c r="AG13" t="str">
         <f>'New vehicle sales'!B69</f>
@@ -4139,113 +4140,113 @@
       <c r="E14" s="19">
         <v>2020</v>
       </c>
-      <c r="F14" s="32">
-        <f>'New vehicle sales'!C19</f>
-        <v>20928</v>
+      <c r="F14" s="43">
+        <f>'New vehicle sales'!C19/1000</f>
+        <v>20.928000000000001</v>
       </c>
       <c r="G14" s="24">
         <f>($F$14*'New vehicle sales'!D43)</f>
-        <v>250.21139742516831</v>
+        <v>0.25021139742516835</v>
       </c>
       <c r="H14" s="24">
         <f>($F$14*'New vehicle sales'!E43)</f>
-        <v>5921.5305667002376</v>
+        <v>5.9215305667002385</v>
       </c>
       <c r="I14" s="24">
         <f>($F$14*'New vehicle sales'!F43)</f>
-        <v>977.88654487264887</v>
+        <v>0.97788654487264892</v>
       </c>
       <c r="J14" s="24">
         <f>($F$14*'New vehicle sales'!G43)</f>
-        <v>436.11637373172033</v>
+        <v>0.43611637373172035</v>
       </c>
       <c r="K14" s="24">
         <f>($F$14*'New vehicle sales'!H43)</f>
-        <v>372.23625953276684</v>
+        <v>0.37223625953276684</v>
       </c>
       <c r="L14" s="24">
         <f>($F$14*'New vehicle sales'!I43)</f>
-        <v>179.63343017914187</v>
+        <v>0.17963343017914188</v>
       </c>
       <c r="M14" s="24">
         <f>($F$14*'New vehicle sales'!J43)</f>
-        <v>566.4344436476041</v>
+        <v>0.56643444364760409</v>
       </c>
       <c r="N14" s="24">
         <f>($F$14*'New vehicle sales'!K43)</f>
-        <v>857.20213235780454</v>
+        <v>0.85720213235780451</v>
       </c>
       <c r="O14" s="24">
         <f>($F$14*'New vehicle sales'!L43)</f>
-        <v>342.63210065804026</v>
+        <v>0.34263210065804023</v>
       </c>
       <c r="P14" s="24">
         <f>($F$14*'New vehicle sales'!M43)</f>
-        <v>390.13675524190597</v>
+        <v>0.390136755241906</v>
       </c>
       <c r="Q14" s="24">
         <f>($F$14*'New vehicle sales'!N43)</f>
-        <v>658.01571779124311</v>
+        <v>0.65801571779124313</v>
       </c>
       <c r="R14" s="24">
         <f>($F$14*'New vehicle sales'!O43)</f>
-        <v>625.94601064918845</v>
+        <v>0.62594601064918842</v>
       </c>
       <c r="S14" s="24">
         <f>($F$14*'New vehicle sales'!P43)</f>
-        <v>522.19081725332364</v>
+        <v>0.52219081725332372</v>
       </c>
       <c r="T14" s="24">
         <f>($F$14*'New vehicle sales'!Q43)</f>
-        <v>2385.8596377679737</v>
+        <v>2.3858596377679739</v>
       </c>
       <c r="U14" s="24">
         <f>($F$14*'New vehicle sales'!R43)</f>
-        <v>649.15996064567105</v>
+        <v>0.64915996064567105</v>
       </c>
       <c r="V14" s="24">
         <f>($F$14*'New vehicle sales'!S43)</f>
-        <v>856.56486943665914</v>
+        <v>0.85656486943665922</v>
       </c>
       <c r="W14" s="24">
         <f>($F$14*'New vehicle sales'!T43)</f>
-        <v>701.22214384490064</v>
+        <v>0.70122214384490067</v>
       </c>
       <c r="X14" s="24">
         <f>($F$14*'New vehicle sales'!U43)</f>
-        <v>510.5838422550824</v>
+        <v>0.51058384225508247</v>
       </c>
       <c r="Y14" s="24">
         <f>($F$14*'New vehicle sales'!V43)</f>
-        <v>1134.1434131374988</v>
+        <v>1.134143413137499</v>
       </c>
       <c r="Z14" s="24">
         <f>($F$14*'New vehicle sales'!W43)</f>
-        <v>140.83071065643387</v>
+        <v>0.14083071065643388</v>
       </c>
       <c r="AA14" s="24">
         <f>($F$14*'New vehicle sales'!X43)</f>
-        <v>573.56739344773496</v>
+        <v>0.573567393447735</v>
       </c>
       <c r="AB14" s="24">
         <f>($F$14*'New vehicle sales'!Y43)</f>
-        <v>283.66550332695255</v>
+        <v>0.28366550332695256</v>
       </c>
       <c r="AC14" s="24">
         <f>($F$14*'New vehicle sales'!Z43)</f>
-        <v>288.02086577422898</v>
+        <v>0.28802086577422903</v>
       </c>
       <c r="AD14" s="24">
         <f>($F$14*'New vehicle sales'!AA43)</f>
-        <v>334.78717435290559</v>
+        <v>0.33478717435290561</v>
       </c>
       <c r="AE14" s="24">
         <f>($F$14*'New vehicle sales'!AB43)</f>
-        <v>699.63557891708342</v>
+        <v>0.69963557891708339</v>
       </c>
       <c r="AF14" s="24">
         <f>($F$14*'New vehicle sales'!AC43)</f>
-        <v>269.78635639607569</v>
+        <v>0.26978635639607573</v>
       </c>
       <c r="AG14" t="str">
         <f>'New vehicle sales'!B107</f>
@@ -4265,113 +4266,113 @@
       <c r="E15" s="19">
         <v>2020</v>
       </c>
-      <c r="F15" s="32">
-        <f>'New vehicle sales'!C20</f>
-        <v>727</v>
+      <c r="F15" s="43">
+        <f>'New vehicle sales'!C20/1000</f>
+        <v>0.72699999999999998</v>
       </c>
       <c r="G15" s="24">
         <f>($F$15*'New vehicle sales'!D43)</f>
-        <v>8.6918810172064873</v>
+        <v>8.6918810172064865E-3</v>
       </c>
       <c r="H15" s="24">
         <f>($F$15*'New vehicle sales'!E43)</f>
-        <v>205.70301615018508</v>
+        <v>0.20570301615018505</v>
       </c>
       <c r="I15" s="24">
         <f>($F$15*'New vehicle sales'!F43)</f>
-        <v>33.969969329243874</v>
+        <v>3.3969969329243871E-2</v>
       </c>
       <c r="J15" s="24">
         <f>($F$15*'New vehicle sales'!G43)</f>
-        <v>15.149875941464101</v>
+        <v>1.51498759414641E-2</v>
       </c>
       <c r="K15" s="24">
         <f>($F$15*'New vehicle sales'!H43)</f>
-        <v>12.930798962171325</v>
+        <v>1.2930798962171324E-2</v>
       </c>
       <c r="L15" s="24">
         <f>($F$15*'New vehicle sales'!I43)</f>
-        <v>6.240133015110672</v>
+        <v>6.2401330151106724E-3</v>
       </c>
       <c r="M15" s="24">
         <f>($F$15*'New vehicle sales'!J43)</f>
-        <v>19.676884581986247</v>
+        <v>1.9676884581986246E-2</v>
       </c>
       <c r="N15" s="24">
         <f>($F$15*'New vehicle sales'!K43)</f>
-        <v>29.777616123094603</v>
+        <v>2.9777616123094604E-2</v>
       </c>
       <c r="O15" s="24">
         <f>($F$15*'New vehicle sales'!L43)</f>
-        <v>11.90240525508387</v>
+        <v>1.190240525508387E-2</v>
       </c>
       <c r="P15" s="24">
         <f>($F$15*'New vehicle sales'!M43)</f>
-        <v>13.552629064452677</v>
+        <v>1.3552629064452678E-2</v>
       </c>
       <c r="Q15" s="24">
         <f>($F$15*'New vehicle sales'!N43)</f>
-        <v>22.858248606375845</v>
+        <v>2.2858248606375847E-2</v>
       </c>
       <c r="R15" s="24">
         <f>($F$15*'New vehicle sales'!O43)</f>
-        <v>21.744206314122707</v>
+        <v>2.1744206314122706E-2</v>
       </c>
       <c r="S15" s="24">
         <f>($F$15*'New vehicle sales'!P43)</f>
-        <v>18.139942858522854</v>
+        <v>1.8139942858522856E-2</v>
       </c>
       <c r="T15" s="24">
         <f>($F$15*'New vehicle sales'!Q43)</f>
-        <v>82.880349610919197</v>
+        <v>8.2880349610919196E-2</v>
       </c>
       <c r="U15" s="24">
         <f>($F$15*'New vehicle sales'!R43)</f>
-        <v>22.550615987643482</v>
+        <v>2.2550615987643484E-2</v>
       </c>
       <c r="V15" s="24">
         <f>($F$15*'New vehicle sales'!S43)</f>
-        <v>29.75547878824786</v>
+        <v>2.9755478788247858E-2</v>
       </c>
       <c r="W15" s="24">
         <f>($F$15*'New vehicle sales'!T43)</f>
-        <v>24.359159908985227</v>
+        <v>2.4359159908985226E-2</v>
       </c>
       <c r="X15" s="24">
         <f>($F$15*'New vehicle sales'!U43)</f>
-        <v>17.736738021762466</v>
+        <v>1.7736738021762469E-2</v>
       </c>
       <c r="Y15" s="24">
         <f>($F$15*'New vehicle sales'!V43)</f>
-        <v>39.39804383366598</v>
+        <v>3.9398043833665984E-2</v>
       </c>
       <c r="Z15" s="24">
         <f>($F$15*'New vehicle sales'!W43)</f>
-        <v>4.8921983298560505</v>
+        <v>4.8921983298560508E-3</v>
       </c>
       <c r="AA15" s="24">
         <f>($F$15*'New vehicle sales'!X43)</f>
-        <v>19.924670060994998</v>
+        <v>1.9924670060994996E-2</v>
       </c>
       <c r="AB15" s="24">
         <f>($F$15*'New vehicle sales'!Y43)</f>
-        <v>9.8540147610232474</v>
+        <v>9.8540147610232456E-3</v>
       </c>
       <c r="AC15" s="24">
         <f>($F$15*'New vehicle sales'!Z43)</f>
-        <v>10.005311994355145</v>
+        <v>1.0005311994355144E-2</v>
       </c>
       <c r="AD15" s="24">
         <f>($F$15*'New vehicle sales'!AA43)</f>
-        <v>11.629887029556688</v>
+        <v>1.1629887029556687E-2</v>
       </c>
       <c r="AE15" s="24">
         <f>($F$15*'New vehicle sales'!AB43)</f>
-        <v>24.304045578780563</v>
+        <v>2.4304045578780561E-2</v>
       </c>
       <c r="AF15" s="24">
         <f>($F$15*'New vehicle sales'!AC43)</f>
-        <v>9.3718788751886013</v>
+        <v>9.3718788751886006E-3</v>
       </c>
       <c r="AG15" t="str">
         <f>'New vehicle sales'!B113</f>
@@ -4392,113 +4393,113 @@
       <c r="E16" s="20">
         <v>2020</v>
       </c>
-      <c r="F16" s="33">
-        <f>'New vehicle sales'!C33</f>
-        <v>2043</v>
+      <c r="F16" s="44">
+        <f>'New vehicle sales'!C33/1000</f>
+        <v>2.0430000000000001</v>
       </c>
       <c r="G16" s="31">
         <f>($F$16*'New vehicle sales'!D43)</f>
-        <v>24.425739914928272</v>
+        <v>2.4425739914928274E-2</v>
       </c>
       <c r="H16" s="31">
         <f>($F$16*'New vehicle sales'!E43)</f>
-        <v>578.06225858985977</v>
+        <v>0.57806225858985982</v>
       </c>
       <c r="I16" s="31">
         <f>($F$16*'New vehicle sales'!F43)</f>
-        <v>95.461688225096609</v>
+        <v>9.5461688225096611E-2</v>
       </c>
       <c r="J16" s="31">
         <f>($F$16*'New vehicle sales'!G43)</f>
-        <v>42.573860451734738</v>
+        <v>4.2573860451734745E-2</v>
       </c>
       <c r="K16" s="31">
         <f>($F$16*'New vehicle sales'!H43)</f>
-        <v>36.337857331108687</v>
+        <v>3.633785733110869E-2</v>
       </c>
       <c r="L16" s="31">
         <f>($F$16*'New vehicle sales'!I43)</f>
-        <v>17.535889614678272</v>
+        <v>1.7535889614678273E-2</v>
       </c>
       <c r="M16" s="31">
         <f>($F$16*'New vehicle sales'!J43)</f>
-        <v>55.295564237961351</v>
+        <v>5.5295564237961357E-2</v>
       </c>
       <c r="N16" s="31">
         <f>($F$16*'New vehicle sales'!K43)</f>
-        <v>83.680426051557461</v>
+        <v>8.3680426051557469E-2</v>
       </c>
       <c r="O16" s="31">
         <f>($F$16*'New vehicle sales'!L43)</f>
-        <v>33.447887119857427</v>
+        <v>3.3447887119857425E-2</v>
       </c>
       <c r="P16" s="31">
         <f>($F$16*'New vehicle sales'!M43)</f>
-        <v>38.08531111234776</v>
+        <v>3.808531111234776E-2</v>
       </c>
       <c r="Q16" s="31">
         <f>($F$16*'New vehicle sales'!N43)</f>
-        <v>64.235766028646296</v>
+        <v>6.4235766028646293E-2</v>
       </c>
       <c r="R16" s="31">
         <f>($F$16*'New vehicle sales'!O43)</f>
-        <v>61.105107977651564</v>
+        <v>6.110510797765157E-2</v>
       </c>
       <c r="S16" s="31">
         <f>($F$16*'New vehicle sales'!P43)</f>
-        <v>50.976483163634377</v>
+        <v>5.097648316363438E-2</v>
       </c>
       <c r="T16" s="31">
         <f>($F$16*'New vehicle sales'!Q43)</f>
-        <v>232.90860282683343</v>
+        <v>0.23290860282683346</v>
       </c>
       <c r="U16" s="31">
         <f>($F$16*'New vehicle sales'!R43)</f>
-        <v>63.371263360049021</v>
+        <v>6.3371263360049016E-2</v>
       </c>
       <c r="V16" s="31">
         <f>($F$16*'New vehicle sales'!S43)</f>
-        <v>83.618216182105058</v>
+        <v>8.3618216182105062E-2</v>
       </c>
       <c r="W16" s="31">
         <f>($F$16*'New vehicle sales'!T43)</f>
-        <v>68.453595177519688</v>
+        <v>6.8453595177519699E-2</v>
       </c>
       <c r="X16" s="31">
         <f>($F$16*'New vehicle sales'!U43)</f>
-        <v>49.843405472435656</v>
+        <v>4.984340547243566E-2</v>
       </c>
       <c r="Y16" s="31">
         <f>($F$16*'New vehicle sales'!V43)</f>
-        <v>110.71554821482752</v>
+        <v>0.11071554821482753</v>
       </c>
       <c r="Z16" s="31">
         <f>($F$16*'New vehicle sales'!W43)</f>
-        <v>13.747952115400153</v>
+        <v>1.3747952115400154E-2</v>
       </c>
       <c r="AA16" s="31">
         <f>($F$16*'New vehicle sales'!X43)</f>
-        <v>55.991885742245913</v>
+        <v>5.5991885742245916E-2</v>
       </c>
       <c r="AB16" s="31">
         <f>($F$16*'New vehicle sales'!Y43)</f>
-        <v>27.691543544388573</v>
+        <v>2.7691543544388575E-2</v>
       </c>
       <c r="AC16" s="31">
         <f>($F$16*'New vehicle sales'!Z43)</f>
-        <v>28.116715824577113</v>
+        <v>2.8116715824577115E-2</v>
       </c>
       <c r="AD16" s="31">
         <f>($F$16*'New vehicle sales'!AA43)</f>
-        <v>32.682062175219137</v>
+        <v>3.2682062175219143E-2</v>
       </c>
       <c r="AE16" s="31">
         <f>($F$16*'New vehicle sales'!AB43)</f>
-        <v>68.298714054262291</v>
+        <v>6.8298714054262299E-2</v>
       </c>
       <c r="AF16" s="31">
         <f>($F$16*'New vehicle sales'!AC43)</f>
-        <v>26.33665549107333</v>
+        <v>2.6336655491073332E-2</v>
       </c>
       <c r="AG16" s="20" t="str">
         <f>'New vehicle sales'!B123</f>
@@ -4575,13 +4576,13 @@
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="33">
         <v>2020</v>
       </c>
     </row>
@@ -4681,13 +4682,13 @@
       <c r="D17" s="12"/>
     </row>
     <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="35">
+      <c r="C18" s="33">
         <v>2020</v>
       </c>
       <c r="D18" s="13"/>
@@ -4809,13 +4810,13 @@
       <c r="C31" s="9"/>
     </row>
     <row r="32" spans="1:4" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="35">
+      <c r="C32" s="33">
         <v>2020</v>
       </c>
     </row>
@@ -5194,628 +5195,628 @@
       <c r="AC44" s="28"/>
     </row>
     <row r="49" spans="2:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="B49" s="43" t="s">
+      <c r="B49" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="C49" s="43"/>
+      <c r="C49" s="41"/>
     </row>
     <row r="50" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="36" t="s">
+      <c r="B50" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="C50" s="36" t="s">
+      <c r="C50" s="34" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="37" t="s">
+      <c r="B51" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="C51" s="38"/>
+      <c r="C51" s="36"/>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B52" s="39" t="s">
+      <c r="B52" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="C52" s="39"/>
+      <c r="C52" s="37"/>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="C53" s="40" t="s">
+      <c r="C53" s="38" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B54" s="40" t="s">
+      <c r="B54" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="C54" s="40" t="s">
+      <c r="C54" s="38" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B55" s="39" t="s">
+      <c r="B55" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="C55" s="39"/>
+      <c r="C55" s="37"/>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B56" s="40" t="s">
+      <c r="B56" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C56" s="40" t="s">
+      <c r="C56" s="38" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B57" s="40" t="s">
+      <c r="B57" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="40" t="s">
+      <c r="C57" s="38" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B58" s="40" t="s">
+      <c r="B58" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="C58" s="40" t="s">
+      <c r="C58" s="38" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B59" s="40" t="s">
+      <c r="B59" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="C59" s="40" t="s">
+      <c r="C59" s="38" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B60" s="40" t="s">
+      <c r="B60" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="C60" s="40" t="s">
+      <c r="C60" s="38" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B61" s="40" t="s">
+      <c r="B61" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="C61" s="40" t="s">
+      <c r="C61" s="38" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B62" s="40" t="s">
+      <c r="B62" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="C62" s="40" t="s">
+      <c r="C62" s="38" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B63" s="40" t="s">
+      <c r="B63" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="C63" s="40" t="s">
+      <c r="C63" s="38" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B64" s="40" t="s">
+      <c r="B64" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="C64" s="40" t="s">
+      <c r="C64" s="38" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B65" s="40" t="s">
+      <c r="B65" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="C65" s="40" t="s">
+      <c r="C65" s="38" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B66" s="40" t="s">
+      <c r="B66" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="C66" s="40" t="s">
+      <c r="C66" s="38" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B67" s="40" t="s">
+      <c r="B67" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="C67" s="40" t="s">
+      <c r="C67" s="38" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B68" s="40" t="s">
+      <c r="B68" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="C68" s="40" t="s">
+      <c r="C68" s="38" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B69" s="40" t="s">
+      <c r="B69" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="C69" s="40" t="s">
+      <c r="C69" s="38" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B70" s="40" t="s">
+      <c r="B70" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="C70" s="40" t="s">
+      <c r="C70" s="38" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B71" s="40" t="s">
+      <c r="B71" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="C71" s="40" t="s">
+      <c r="C71" s="38" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B72" s="40" t="s">
+      <c r="B72" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="C72" s="40" t="s">
+      <c r="C72" s="38" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B73" s="40" t="s">
+      <c r="B73" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="C73" s="40" t="s">
+      <c r="C73" s="38" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B74" s="40" t="s">
+      <c r="B74" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="C74" s="40" t="s">
+      <c r="C74" s="38" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B75" s="39" t="s">
+      <c r="B75" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="C75" s="39"/>
+      <c r="C75" s="37"/>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B76" s="40" t="s">
+      <c r="B76" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="C76" s="40" t="s">
+      <c r="C76" s="38" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B77" s="40" t="s">
+      <c r="B77" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="C77" s="40" t="s">
+      <c r="C77" s="38" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B78" s="40" t="s">
+      <c r="B78" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="C78" s="40" t="s">
+      <c r="C78" s="38" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B79" s="40" t="s">
+      <c r="B79" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="C79" s="40" t="s">
+      <c r="C79" s="38" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B80" s="40" t="s">
+      <c r="B80" s="38" t="s">
         <v>147</v>
       </c>
-      <c r="C80" s="40" t="s">
+      <c r="C80" s="38" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B81" s="40" t="s">
+      <c r="B81" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="C81" s="40" t="s">
+      <c r="C81" s="38" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B82" s="40" t="s">
+      <c r="B82" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="C82" s="40" t="s">
+      <c r="C82" s="38" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B83" s="40" t="s">
+      <c r="B83" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="C83" s="40" t="s">
+      <c r="C83" s="38" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B84" s="40" t="s">
+      <c r="B84" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="C84" s="40" t="s">
+      <c r="C84" s="38" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B85" s="40" t="s">
+      <c r="B85" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="C85" s="40" t="s">
+      <c r="C85" s="38" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B86" s="40" t="s">
+      <c r="B86" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="C86" s="40" t="s">
+      <c r="C86" s="38" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B87" s="40" t="s">
+      <c r="B87" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="C87" s="40" t="s">
+      <c r="C87" s="38" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B88" s="40" t="s">
+      <c r="B88" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="C88" s="40" t="s">
+      <c r="C88" s="38" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B89" s="40" t="s">
+      <c r="B89" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="C89" s="40" t="s">
+      <c r="C89" s="38" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B90" s="40" t="s">
+      <c r="B90" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="C90" s="40" t="s">
+      <c r="C90" s="38" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B91" s="40" t="s">
+      <c r="B91" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="C91" s="40" t="s">
+      <c r="C91" s="38" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B92" s="40" t="s">
+      <c r="B92" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="C92" s="40" t="s">
+      <c r="C92" s="38" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B93" s="40" t="s">
+      <c r="B93" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="C93" s="40" t="s">
+      <c r="C93" s="38" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B94" s="40" t="s">
+      <c r="B94" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="C94" s="40" t="s">
+      <c r="C94" s="38" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B95" s="39" t="s">
+      <c r="B95" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="C95" s="39"/>
+      <c r="C95" s="37"/>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B96" s="40" t="s">
+      <c r="B96" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="C96" s="40" t="s">
+      <c r="C96" s="38" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B97" s="40" t="s">
+      <c r="B97" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="C97" s="40" t="s">
+      <c r="C97" s="38" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B98" s="40" t="s">
+      <c r="B98" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="C98" s="40" t="s">
+      <c r="C98" s="38" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B99" s="40" t="s">
+      <c r="B99" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="C99" s="40" t="s">
+      <c r="C99" s="38" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B100" s="40" t="s">
+      <c r="B100" s="38" t="s">
         <v>186</v>
       </c>
-      <c r="C100" s="40" t="s">
+      <c r="C100" s="38" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B101" s="39" t="s">
+      <c r="B101" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="C101" s="39"/>
+      <c r="C101" s="37"/>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B102" s="40" t="s">
+      <c r="B102" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="C102" s="40" t="s">
+      <c r="C102" s="38" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B103" s="40" t="s">
+      <c r="B103" s="38" t="s">
         <v>191</v>
       </c>
-      <c r="C103" s="40" t="s">
+      <c r="C103" s="38" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B104" s="40" t="s">
+      <c r="B104" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="C104" s="40" t="s">
+      <c r="C104" s="38" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B105" s="41" t="s">
+      <c r="B105" s="39" t="s">
         <v>195</v>
       </c>
-      <c r="C105" s="42"/>
+      <c r="C105" s="40"/>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B106" s="39" t="s">
+      <c r="B106" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="C106" s="39"/>
+      <c r="C106" s="37"/>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B107" s="40" t="s">
+      <c r="B107" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="C107" s="40" t="s">
+      <c r="C107" s="38" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B108" s="40" t="s">
+      <c r="B108" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="C108" s="40" t="s">
+      <c r="C108" s="38" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B109" s="40" t="s">
+      <c r="B109" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="C109" s="40" t="s">
+      <c r="C109" s="38" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B110" s="40" t="s">
+      <c r="B110" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="C110" s="40" t="s">
+      <c r="C110" s="38" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B111" s="40" t="s">
+      <c r="B111" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="C111" s="40" t="s">
+      <c r="C111" s="38" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B112" s="40" t="s">
+      <c r="B112" s="38" t="s">
         <v>207</v>
       </c>
-      <c r="C112" s="40" t="s">
+      <c r="C112" s="38" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B113" s="40" t="s">
+      <c r="B113" s="38" t="s">
         <v>209</v>
       </c>
-      <c r="C113" s="40" t="s">
+      <c r="C113" s="38" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B114" s="39" t="s">
+      <c r="B114" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="C114" s="39"/>
+      <c r="C114" s="37"/>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B115" s="40" t="s">
+      <c r="B115" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="C115" s="40" t="s">
+      <c r="C115" s="38" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B116" s="40" t="s">
+      <c r="B116" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="C116" s="40" t="s">
+      <c r="C116" s="38" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B117" s="40" t="s">
+      <c r="B117" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="C117" s="40" t="s">
+      <c r="C117" s="38" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B118" s="40" t="s">
+      <c r="B118" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="C118" s="40" t="s">
+      <c r="C118" s="38" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B119" s="40" t="s">
+      <c r="B119" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="C119" s="40" t="s">
+      <c r="C119" s="38" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B120" s="40" t="s">
+      <c r="B120" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="C120" s="40" t="s">
+      <c r="C120" s="38" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B121" s="40" t="s">
+      <c r="B121" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="C121" s="40" t="s">
+      <c r="C121" s="38" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B122" s="39" t="s">
+      <c r="B122" s="37" t="s">
         <v>226</v>
       </c>
-      <c r="C122" s="39"/>
+      <c r="C122" s="37"/>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B123" s="40" t="s">
+      <c r="B123" s="38" t="s">
         <v>227</v>
       </c>
-      <c r="C123" s="40" t="s">
+      <c r="C123" s="38" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B124" s="40" t="s">
+      <c r="B124" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="C124" s="40" t="s">
+      <c r="C124" s="38" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B125" s="40" t="s">
+      <c r="B125" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="C125" s="40" t="s">
+      <c r="C125" s="38" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B126" s="40" t="s">
+      <c r="B126" s="38" t="s">
         <v>233</v>
       </c>
-      <c r="C126" s="40" t="s">
+      <c r="C126" s="38" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B127" s="40" t="s">
+      <c r="B127" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="C127" s="40" t="s">
+      <c r="C127" s="38" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B128" s="40" t="s">
+      <c r="B128" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="C128" s="40" t="s">
+      <c r="C128" s="38" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B129" s="40" t="s">
+      <c r="B129" s="38" t="s">
         <v>239</v>
       </c>
-      <c r="C129" s="40" t="s">
+      <c r="C129" s="38" t="s">
         <v>240</v>
       </c>
     </row>

</xml_diff>